<commit_message>
Modify ESP8266 code for more stable - Config mode: fix issue that config params are stored wrongly in EEPROM - Only call handleClient() when at least 1 client connect to ESP server - Add an extended command to connect to WiFi
Signed-off-by: lvminh97 <lvminh97@gmail.com>
</commit_message>
<xml_diff>
--- a/00.Docs/Design doc.xlsx
+++ b/00.Docs/Design doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\PatientCare\00.Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\DOAN\PatientCare\00.Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86523E01-3809-4B94-AD06-421C28EF0B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7EF3E-43CD-486C-A2AC-6B5D2C82E17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPIO" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
   <si>
     <t>GPIO</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>Return the Wifi status of ESP8266</t>
+  </si>
+  <si>
+    <t>84 F0 80 85</t>
+  </si>
+  <si>
+    <t>Connect to WiFi</t>
   </si>
 </sst>
 </file>
@@ -851,10 +857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D38DBF2-EA9B-4572-BEFD-3C36D31E9AD9}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -929,67 +935,78 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Remove delay time when getting command from buffer: add 2 bytes 84 F1 for marking the end of command - Move the display of DHT11 and LM35 sensor values to before MAX30100 - Add new command to send the value of LM35: now LM35 value is not sent with MAX30100 values - Resize the command buffer of MCU to 40 bytes
Signed-off-by: lvminh97 <lvminh97@gmail.com>
</commit_message>
<xml_diff>
--- a/00.Docs/Design doc.xlsx
+++ b/00.Docs/Design doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\DOAN\PatientCare\00.Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7EF3E-43CD-486C-A2AC-6B5D2C82E17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550A6BE6-BF4D-4478-A727-9D92768A83A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>GPIO</t>
   </si>
@@ -187,27 +187,15 @@
     <t>ESP -&gt; MCU</t>
   </si>
   <si>
-    <t>Send Heart rate XXXX, SpO2 YY and body temperature ZZ</t>
-  </si>
-  <si>
     <t>Send DHT11 values: temperature XX and humidity YY</t>
   </si>
   <si>
-    <t>84 F0 80 81</t>
-  </si>
-  <si>
     <t>Start wifi configuration mode</t>
   </si>
   <si>
-    <t>84 F0 80 82</t>
-  </si>
-  <si>
     <t>Stop wifi configuration mode</t>
   </si>
   <si>
-    <t>84 F0 80 83</t>
-  </si>
-  <si>
     <t>Reset ESP8266</t>
   </si>
   <si>
@@ -217,46 +205,64 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>84 F0 81 82</t>
-  </si>
-  <si>
     <t>Finish wifi configuration</t>
   </si>
   <si>
-    <t>84 F0 82 81 XX YY</t>
-  </si>
-  <si>
-    <t>84 F0 82 82 XX XX YY ZZ</t>
-  </si>
-  <si>
-    <t>84 F0 83 XX YY</t>
-  </si>
-  <si>
     <t>Send the status of Relay 1 (XX) and Relay 2 (YY)</t>
   </si>
   <si>
-    <t>84 F0 82 83 XX</t>
-  </si>
-  <si>
     <t>Send the SOS status XX</t>
   </si>
   <si>
-    <t>84 F0 80 84</t>
-  </si>
-  <si>
     <t>Get Wifi status of ESP8266</t>
   </si>
   <si>
-    <t>84 F0 81 84 XX</t>
-  </si>
-  <si>
     <t>Return the Wifi status of ESP8266</t>
   </si>
   <si>
-    <t>84 F0 80 85</t>
-  </si>
-  <si>
     <t>Connect to WiFi</t>
+  </si>
+  <si>
+    <t>Send the body temperature XX</t>
+  </si>
+  <si>
+    <t>Send Heart rate XXXX, SpO2 YY</t>
+  </si>
+  <si>
+    <t>84 F0 80 81 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 80 82 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 80 83 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 80 84 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 80 85 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 81 82 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 81 84 XX 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 82 81 XX YY 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 82 82 XX XX YY 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 82 83 XX 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 82 84 XX 84 F1</t>
+  </si>
+  <si>
+    <t>84 F0 83 XX YY 84 F1</t>
   </si>
 </sst>
 </file>
@@ -857,10 +863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D38DBF2-EA9B-4572-BEFD-3C36D31E9AD9}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -883,76 +889,76 @@
         <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,51 +969,62 @@
         <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>68</v>
+      <c r="C13" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>